<commit_message>
added more data from map server, and included two W 132nd street lots, one of them empty.
</commit_message>
<xml_diff>
--- a/building-info.xlsx
+++ b/building-info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="74">
   <si>
     <t>Building</t>
   </si>
@@ -129,9 +129,6 @@
     <t>01998-0029</t>
   </si>
   <si>
-    <t>39,766 (over allowable)</t>
-  </si>
-  <si>
     <t>605 W 131st St.</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Brownfield Site,Air Discharge Facility,Hazardous Waste Violation</t>
   </si>
   <si>
-    <t>140,229 (over allowable)</t>
-  </si>
-  <si>
     <t>635 W 131st St.</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>01998-0013</t>
   </si>
   <si>
-    <t>1,049 (over allowable)</t>
-  </si>
-  <si>
     <t>641 W 131st St.</t>
   </si>
   <si>
@@ -229,6 +220,24 @@
   </si>
   <si>
     <t>Max Flr Area Ratio</t>
+  </si>
+  <si>
+    <t>Floors</t>
+  </si>
+  <si>
+    <t>640 W 132nd St.</t>
+  </si>
+  <si>
+    <t>624 W 132nd St.</t>
+  </si>
+  <si>
+    <t>C6-1</t>
+  </si>
+  <si>
+    <t>01998-0057</t>
+  </si>
+  <si>
+    <t>01998-0049</t>
   </si>
 </sst>
 </file>
@@ -238,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -248,6 +257,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -273,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -283,6 +298,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,98 +594,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="1.5703125" customWidth="1"/>
-    <col min="4" max="4" width="1" style="1" customWidth="1"/>
-    <col min="5" max="6" width="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="1" customWidth="1"/>
-    <col min="11" max="11" width="1.5703125" customWidth="1"/>
-    <col min="12" max="14" width="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="14" width="1.7109375" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
     <col min="16" max="16" width="1.85546875" customWidth="1"/>
     <col min="17" max="17" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="V1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="W1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="33" customHeight="1">
+    </row>
+    <row r="2" spans="1:23" ht="33" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -711,8 +730,8 @@
       <c r="N2" s="6">
         <v>29973</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>37</v>
+      <c r="O2" s="7">
+        <v>-39766</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>26</v>
@@ -729,16 +748,25 @@
       <c r="T2">
         <v>19983</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="27.75" customHeight="1">
+      <c r="U2">
+        <v>79708</v>
+      </c>
+      <c r="V2">
+        <v>6</v>
+      </c>
+      <c r="W2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="27.75" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -791,16 +819,25 @@
       <c r="T3">
         <v>4996</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="27.75" customHeight="1">
+      <c r="U3">
+        <v>4996</v>
+      </c>
+      <c r="V3">
+        <v>6</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="27.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>4</v>
@@ -827,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>8</v>
@@ -853,16 +890,25 @@
       <c r="T4">
         <v>9992</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="27.75" customHeight="1">
+      <c r="U4">
+        <v>9992</v>
+      </c>
+      <c r="V4">
+        <v>6</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="27.75" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>4</v>
@@ -889,7 +935,7 @@
         <v>34</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M5" s="5">
         <v>18603127</v>
@@ -897,8 +943,8 @@
       <c r="N5" s="8">
         <v>39261</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>49</v>
+      <c r="O5" s="7">
+        <v>-140229</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>26</v>
@@ -915,16 +961,25 @@
       <c r="T5">
         <v>34970</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="27.75" customHeight="1">
+      <c r="U5">
+        <v>210000</v>
+      </c>
+      <c r="V5">
+        <v>6</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="27.75" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -959,8 +1014,8 @@
       <c r="N6" s="8">
         <v>39261</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>53</v>
+      <c r="O6" s="7">
+        <v>-1049</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>26</v>
@@ -983,16 +1038,19 @@
       <c r="V6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="29.25" customHeight="1">
+      <c r="W6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="29.25" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>4</v>
@@ -1051,16 +1109,19 @@
       <c r="V7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="29.25" customHeight="1">
+      <c r="W7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="29.25" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1119,16 +1180,19 @@
       <c r="V8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="36.75" customHeight="1">
+      <c r="W8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="36.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
@@ -1172,16 +1236,34 @@
       <c r="Q9" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="36.75" customHeight="1">
+      <c r="R9">
+        <v>69.92</v>
+      </c>
+      <c r="S9">
+        <v>100</v>
+      </c>
+      <c r="T9">
+        <v>6992</v>
+      </c>
+      <c r="U9">
+        <v>8588</v>
+      </c>
+      <c r="V9">
+        <v>6</v>
+      </c>
+      <c r="W9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="36.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -1225,23 +1307,131 @@
       <c r="Q10" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="R10">
+        <v>99.92</v>
+      </c>
+      <c r="S10">
+        <v>100</v>
+      </c>
+      <c r="T10">
+        <v>9992</v>
+      </c>
+      <c r="U10">
+        <v>19984</v>
+      </c>
+      <c r="V10">
+        <v>6</v>
+      </c>
+      <c r="W10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="E11" s="5">
+        <v>146250</v>
+      </c>
+      <c r="F11" s="5">
+        <v>253350</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="7">
+        <v>12490</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11">
+        <v>99.92</v>
+      </c>
+      <c r="S11">
+        <v>100</v>
+      </c>
+      <c r="T11">
+        <v>9992</v>
+      </c>
+      <c r="U11">
+        <v>7500</v>
+      </c>
+      <c r="V11">
+        <v>6</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7">
+        <v>39968</v>
+      </c>
+      <c r="P12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12">
+        <v>99.92</v>
+      </c>
+      <c r="S12">
+        <v>200</v>
+      </c>
+      <c r="T12">
+        <v>19984</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>6</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:23">
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:23">
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:23">
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="4:4">
@@ -1250,7 +1440,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>